<commit_message>
remove old direcotry with uncorrect name
</commit_message>
<xml_diff>
--- a/Weekly Tasks Folder/21.02.2016 - 27.02.2016/Олимов_Заир.xlsx
+++ b/Weekly Tasks Folder/21.02.2016 - 27.02.2016/Олимов_Заир.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
-    <t>План на неделю с 20.02.16  по 27.02.16    </t>
+    <t>План на неделю с 20.02.16  по 27.02.16</t>
   </si>
   <si>
     <t>Общая задача: Настройка HLS и настройка nginx reverse proxy</t>
@@ -62,9 +62,10 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="6">
-    <font>
-      <name val="Arial"/>
+  <fonts count="8">
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -97,8 +98,22 @@
       <color rgb="00FFFF00"/>
       <sz val="11"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="0000FF00"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="00008000"/>
+      <sz val="10"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,8 +122,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
-        <bgColor rgb="00FFFF00"/>
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0033CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00008000"/>
+        <bgColor rgb="00008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -121,10 +148,10 @@
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <left style="thick"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
       <diagonal/>
     </border>
   </borders>
@@ -153,7 +180,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -161,8 +188,12 @@
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="6" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="7" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="4" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -183,16 +214,16 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="D5" activeCellId="0" pane="topLeft" sqref="D5"/>
+      <selection activeCell="H8" activeCellId="0" pane="topLeft" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5450980392157"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6627450980392"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -205,7 +236,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -218,7 +249,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -245,7 +276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="4">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -258,46 +289,46 @@
       <c r="H4" s="4"/>
       <c r="I4" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="5">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+      <c r="I5" s="6"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="6"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
       <c r="I6" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -305,9 +336,9 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="2"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="10"/>
       <c r="I8" s="2"/>
     </row>
   </sheetData>
@@ -338,17 +369,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -363,17 +394,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>